<commit_message>
updated scraping function 400 to 490 datapoints
</commit_message>
<xml_diff>
--- a/stockx_scraper-master/prods.xlsx
+++ b/stockx_scraper-master/prods.xlsx
@@ -43,27 +43,27 @@
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-cinder</t>
   </si>
   <si>
+    <t>https://stockx.com//adidas-yeezy-boost-350-v2-white-core-black-red</t>
+  </si>
+  <si>
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-desert-sage</t>
   </si>
   <si>
-    <t>https://stockx.com//adidas-yeezy-boost-350-v2-white-core-black-red</t>
-  </si>
-  <si>
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-yecheil</t>
   </si>
   <si>
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-earth</t>
   </si>
   <si>
+    <t>https://stockx.com//adidas-yeezy-boost-350-v2-cream-white</t>
+  </si>
+  <si>
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-yeezreel</t>
   </si>
   <si>
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-tail-light</t>
   </si>
   <si>
-    <t>https://stockx.com//adidas-yeezy-boost-350-v2-cream-white</t>
-  </si>
-  <si>
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-citrin</t>
   </si>
   <si>
@@ -82,12 +82,12 @@
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-sulfur</t>
   </si>
   <si>
+    <t>https://stockx.com//adidas-yeezy-boost-350-v2-yeshaya</t>
+  </si>
+  <si>
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-clay</t>
   </si>
   <si>
-    <t>https://stockx.com//adidas-yeezy-boost-350-v2-yeshaya</t>
-  </si>
-  <si>
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-static</t>
   </si>
   <si>
@@ -124,18 +124,18 @@
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-core-black-red-2017</t>
   </si>
   <si>
+    <t>https://stockx.com//adidas-yeezy-boost-350-v2-core-black-red</t>
+  </si>
+  <si>
+    <t>https://stockx.com//adidas-yeezy-boost-350-turtledove</t>
+  </si>
+  <si>
+    <t>https://stockx.com//adidas-yeezy-boost-350-v2-flax</t>
+  </si>
+  <si>
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-true-form</t>
   </si>
   <si>
-    <t>https://stockx.com//adidas-yeezy-boost-350-v2-flax</t>
-  </si>
-  <si>
-    <t>https://stockx.com//adidas-yeezy-boost-350-v2-core-black-red</t>
-  </si>
-  <si>
-    <t>https://stockx.com//adidas-yeezy-boost-350-turtledove</t>
-  </si>
-  <si>
     <t>https://stockx.com//adidas-yeezy-boost-350-v2-hyperspace</t>
   </si>
   <si>
@@ -163,27 +163,27 @@
     <t>adidas Yeezy Boost 350 V2 Cinder</t>
   </si>
   <si>
+    <t>adidas Yeezy Boost 350 V2 Zebra</t>
+  </si>
+  <si>
     <t>adidas Yeezy Boost 350 V2 Desert Sage</t>
   </si>
   <si>
-    <t>adidas Yeezy Boost 350 V2 Zebra</t>
-  </si>
-  <si>
     <t>adidas Yeezy Boost 350 V2 Yecheil (Non-Reflective)</t>
   </si>
   <si>
     <t>adidas Yeezy Boost 350 V2 Earth</t>
   </si>
   <si>
+    <t>adidas Yeezy Boost 350 V2 Cream/Triple White</t>
+  </si>
+  <si>
     <t>adidas Yeezy Boost 350 V2 Yeezreel (Non-Reflective)</t>
   </si>
   <si>
     <t>adidas Yeezy Boost 350 V2 Tail Light</t>
   </si>
   <si>
-    <t>adidas Yeezy Boost 350 V2 Cream/Triple White</t>
-  </si>
-  <si>
     <t>adidas Yeezy Boost 350 V2 Citrin (Non-Reflective)</t>
   </si>
   <si>
@@ -202,12 +202,12 @@
     <t>adidas Yeezy Boost 350 V2 Sulfur</t>
   </si>
   <si>
+    <t>adidas Yeezy Boost 350 V2 Yeshaya (Non-Reflective)</t>
+  </si>
+  <si>
     <t>adidas Yeezy Boost 350 V2 Clay</t>
   </si>
   <si>
-    <t>adidas Yeezy Boost 350 V2 Yeshaya (Non-Reflective)</t>
-  </si>
-  <si>
     <t>adidas Yeezy Boost 350 V2 Static (Non-Reflective)</t>
   </si>
   <si>
@@ -244,18 +244,18 @@
     <t>adidas Yeezy Boost 350 V2 Black Red</t>
   </si>
   <si>
+    <t>adidas Yeezy Boost 350 V2 Core Black Red</t>
+  </si>
+  <si>
+    <t>adidas Yeezy Boost 350 Turtledove</t>
+  </si>
+  <si>
+    <t>adidas Yeezy Boost 350 V2 Flax</t>
+  </si>
+  <si>
     <t>adidas Yeezy Boost 350 V2 Trfrm</t>
   </si>
   <si>
-    <t>adidas Yeezy Boost 350 V2 Flax</t>
-  </si>
-  <si>
-    <t>adidas Yeezy Boost 350 V2 Core Black Red</t>
-  </si>
-  <si>
-    <t>adidas Yeezy Boost 350 Turtledove</t>
-  </si>
-  <si>
     <t>adidas Yeezy Boost 350 V2 Hyperspace</t>
   </si>
   <si>
@@ -283,27 +283,27 @@
     <t xml:space="preserve"> FY2903 </t>
   </si>
   <si>
+    <t xml:space="preserve"> CP9654 </t>
+  </si>
+  <si>
     <t xml:space="preserve"> FX9035 </t>
   </si>
   <si>
-    <t xml:space="preserve"> CP9654 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> FW5190 </t>
   </si>
   <si>
     <t xml:space="preserve"> FX9033 </t>
   </si>
   <si>
+    <t xml:space="preserve"> CP9366 </t>
+  </si>
+  <si>
     <t xml:space="preserve"> FW5191 </t>
   </si>
   <si>
     <t xml:space="preserve"> FX9017 </t>
   </si>
   <si>
-    <t xml:space="preserve"> CP9366 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> FW3042 </t>
   </si>
   <si>
@@ -322,12 +322,12 @@
     <t xml:space="preserve"> FY5346 </t>
   </si>
   <si>
+    <t xml:space="preserve"> FX4348 </t>
+  </si>
+  <si>
     <t xml:space="preserve"> EG7490 </t>
   </si>
   <si>
-    <t xml:space="preserve"> FX4348 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> EF2905 </t>
   </si>
   <si>
@@ -364,18 +364,18 @@
     <t xml:space="preserve"> CP9652 </t>
   </si>
   <si>
+    <t xml:space="preserve"> BY9612 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AQ4832 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FX9028 </t>
+  </si>
+  <si>
     <t xml:space="preserve"> EG7492 </t>
   </si>
   <si>
-    <t xml:space="preserve"> FX9028 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BY9612 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AQ4832 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> EG7491 </t>
   </si>
   <si>
@@ -433,12 +433,12 @@
     <t xml:space="preserve"> Sulfur/Sulfur/Sulfur </t>
   </si>
   <si>
+    <t xml:space="preserve"> Yeshaya/Yeshaya/Yeshaya </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Clay/Clay/Clay </t>
   </si>
   <si>
-    <t xml:space="preserve"> Yeshaya/Yeshaya/Yeshaya </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Static/Static/Static </t>
   </si>
   <si>
@@ -460,12 +460,12 @@
     <t xml:space="preserve"> Synth/Synth/Synth </t>
   </si>
   <si>
+    <t xml:space="preserve"> Flax/Flax/Flax </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Grey/Grey/Grey </t>
   </si>
   <si>
-    <t xml:space="preserve"> Flax/Flax/Flax </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Natural/Natural/Natural </t>
   </si>
   <si>
@@ -493,24 +493,24 @@
     <t xml:space="preserve"> 03/21/2020 </t>
   </si>
   <si>
+    <t xml:space="preserve"> 02/25/2017 </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 03/14/2020 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 02/25/2017 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 12/20/2019 </t>
   </si>
   <si>
     <t xml:space="preserve"> 02/22/2020 </t>
   </si>
   <si>
+    <t xml:space="preserve"> 04/29/2017 </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 12/14/2019 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 04/29/2017 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 09/23/2019 </t>
   </si>
   <si>
@@ -529,12 +529,12 @@
     <t xml:space="preserve"> 05/09/2020 </t>
   </si>
   <si>
+    <t xml:space="preserve"> 01/25/2020 </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 03/30/2019 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 01/25/2020 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 12/27/2018 </t>
   </si>
   <si>
@@ -568,13 +568,13 @@
     <t xml:space="preserve"> 02/11/2017 </t>
   </si>
   <si>
+    <t xml:space="preserve"> 11/23/2016 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 06/27/2015 </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 03/16/2019 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11/23/2016 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 06/27/2015 </t>
   </si>
   <si>
     <t xml:space="preserve"> 11/14/2015 </t>
@@ -1068,9 +1068,6 @@
       <c r="D5" t="s">
         <v>89</v>
       </c>
-      <c r="E5" t="s">
-        <v>129</v>
-      </c>
       <c r="F5" t="s">
         <v>153</v>
       </c>
@@ -1091,6 +1088,9 @@
       <c r="D6" t="s">
         <v>90</v>
       </c>
+      <c r="E6" t="s">
+        <v>129</v>
+      </c>
       <c r="F6" t="s">
         <v>153</v>
       </c>
@@ -1157,9 +1157,6 @@
       <c r="D9" t="s">
         <v>93</v>
       </c>
-      <c r="E9" t="s">
-        <v>132</v>
-      </c>
       <c r="F9" t="s">
         <v>153</v>
       </c>
@@ -1181,13 +1178,13 @@
         <v>94</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F10" t="s">
         <v>153</v>
       </c>
       <c r="G10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1203,11 +1200,14 @@
       <c r="D11" t="s">
         <v>95</v>
       </c>
+      <c r="E11" t="s">
+        <v>133</v>
+      </c>
       <c r="F11" t="s">
         <v>153</v>
       </c>
       <c r="G11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1668,9 +1668,6 @@
       <c r="D32" t="s">
         <v>116</v>
       </c>
-      <c r="E32" t="s">
-        <v>148</v>
-      </c>
       <c r="F32" t="s">
         <v>153</v>
       </c>
@@ -1691,14 +1688,11 @@
       <c r="D33" t="s">
         <v>117</v>
       </c>
-      <c r="E33" t="s">
-        <v>149</v>
-      </c>
       <c r="F33" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G33" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1714,11 +1708,14 @@
       <c r="D34" t="s">
         <v>118</v>
       </c>
+      <c r="E34" t="s">
+        <v>148</v>
+      </c>
       <c r="F34" t="s">
         <v>153</v>
       </c>
       <c r="G34" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1734,8 +1731,11 @@
       <c r="D35" t="s">
         <v>119</v>
       </c>
+      <c r="E35" t="s">
+        <v>149</v>
+      </c>
       <c r="F35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G35" t="s">
         <v>186</v>
@@ -1755,13 +1755,13 @@
         <v>120</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F36" t="s">
         <v>153</v>
       </c>
       <c r="G36" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:7">

</xml_diff>